<commit_message>
Actualización guiones, guías didácticas y solicitudes gráficas.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion04/SolicitudGrafica_CN_10_04.xlsx
+++ b/fuentes/contenidos/grado10/guion04/SolicitudGrafica_CN_10_04.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="0" windowWidth="13140" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="13760" yWindow="0" windowWidth="11840" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="235">
   <si>
     <t>Fecha:</t>
   </si>
@@ -650,9 +650,6 @@
     <t>Fuerza de los libros apoyados sobre la mesa</t>
   </si>
   <si>
-    <t>Características de la fuerza</t>
-  </si>
-  <si>
     <t>Fuerzas colineales</t>
   </si>
   <si>
@@ -704,27 +701,6 @@
     <t>Fuerza normal sobre un libro apoyado en una mesa</t>
   </si>
   <si>
-    <t>Fuerzas que actuan sobre un plano inclinado</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/3/39/GodfreyKneller-IsaacNewton-1689.jpg</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/0/0e/Parallel_net_force01.jpg</t>
-  </si>
-  <si>
-    <t>http://www.texample.net/media/tikz/examples/PNG/free-body-diagrams.png</t>
-  </si>
-  <si>
-    <t>Isaac Newton</t>
-  </si>
-  <si>
-    <t>Fuerzas en equilibrio: Primera Ley de Newton</t>
-  </si>
-  <si>
-    <t>Desequilibrio de fuerzas: Segunda Ley de Newton</t>
-  </si>
-  <si>
     <t>Imagen adaptada: cambiar la letra P por la letra W, conservando los subíndices. También se debe alargar la flecha que al lado del Wx. Revisar muestra con cambios,</t>
   </si>
   <si>
@@ -737,84 +713,25 @@
     <t>Cambiar la letra P por W conservando los subíndices 1 y 2.</t>
   </si>
   <si>
-    <t>Imagen con adaptación del autor, revisar muestra</t>
-  </si>
-  <si>
-    <t>Fuerza neta obtenida gráficamente 1</t>
-  </si>
-  <si>
-    <t>Fuerza neta obtenida gráficamente 2</t>
-  </si>
-  <si>
-    <t>Cambios como en el anterior, revisar muestra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imagen adaptada: Agregar y modificar las letras que se indican 
-Los vectores (flechas) N y Wy deben quedar de la misma longitud.
-Los vectores (flechas) T y Wx deben quedar de la misma longitud. Revisar muestra
-</t>
-  </si>
-  <si>
-    <t>Tercera ley de Newton: Ley de acción-reacción</t>
-  </si>
-  <si>
-    <t>4° ESO/Física y Química/La dinámica/2. Las leyes de Newton/2.3 La tercera ley de Newton o ley de acción y reacción</t>
-  </si>
-  <si>
-    <t>Funcionamiento de un cohete: Tercera ley de Newton</t>
-  </si>
-  <si>
-    <t>Aceleración centrípeta</t>
-  </si>
-  <si>
-    <t>4° ESO/ Física y química/La dinámica/5. La fuerza centrípeta</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/f/ff/Breaking_String.PNG</t>
-  </si>
-  <si>
-    <t>Fuerza centrípeta en ruptura de cuerda en movimiento circular</t>
-  </si>
-  <si>
-    <t>Cambiar las palabras de inglés a español:
-Velocity por velocidad
-Centripetal forcé por Fuerza centrípeta</t>
-  </si>
-  <si>
-    <t>Fuerza centrípeta en pista circular</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/4/40/US_Navy_040501-N-1336S-037_The_U.S._Navy_sponsored_Chevy_Monte_Carlo_NASCAR_leads_a_pack_into_turn_four_at_California_Speedway.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Par de fuerzas </t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/4/48/Par_de_fuerzas.jpg</t>
-  </si>
-  <si>
-    <t>Producto vectorial o producto cruz</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/4/4e/Cross_product_parallelogram.svg</t>
-  </si>
-  <si>
-    <t>Torque: Principio de la balanza</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/c/c3/Lever_Principle_3D.png</t>
-  </si>
-  <si>
-    <t>quitar la ecuación  y poner la letra O. Revisar muestra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palancas y su clasificación </t>
-  </si>
-  <si>
-    <t>4°ESO/Física y química/La fuerza/3. Fuerzas en equilibrio/ 3.1 El equilibrio en máquinas simples: la palanca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funcionamiento palanca de primer género  </t>
+    <t>Elementos del vector fuerza</t>
+  </si>
+  <si>
+    <t>https://pixabay.com/es/tierra-planeta-azul-globo-luna-11007/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuerza gravitacional entre la Tierra y la Luna </t>
+  </si>
+  <si>
+    <t>Creada por autor, ilustrar</t>
+  </si>
+  <si>
+    <t>uerza normal sobre un libro apoyado en una mesa</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/56380734@N05/5401199351</t>
+  </si>
+  <si>
+    <t>Polea</t>
   </si>
 </sst>
 </file>
@@ -1480,8 +1397,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1802,6 +1741,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1900,12 +1843,8 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="123">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1956,6 +1895,17 @@
     <cellStyle name="Hipervínculo" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -2006,6 +1956,17 @@
     <cellStyle name="Hipervínculo visitado" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -2693,8 +2654,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="9" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2740,14 +2701,14 @@
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="F2" s="77" t="s">
+      <c r="D2" s="86"/>
+      <c r="F2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="78"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2771,14 +2732,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="87">
         <v>10</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="F3" s="79">
+      <c r="D3" s="88"/>
+      <c r="F3" s="80">
         <v>42144</v>
       </c>
-      <c r="G3" s="80"/>
+      <c r="G3" s="81"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2802,10 +2763,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -2834,10 +2795,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="89"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2921,12 +2882,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="84"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -2991,7 +2952,7 @@
         <v>192</v>
       </c>
       <c r="C10" s="20" t="str">
-        <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C10:C18" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="63" t="s">
@@ -3081,7 +3042,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E12" s="63" t="s">
         <v>153</v>
@@ -3103,7 +3064,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="64" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
@@ -3146,7 +3107,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
@@ -3167,7 +3128,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E14" s="63" t="s">
         <v>153</v>
@@ -3189,7 +3150,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
@@ -3210,7 +3171,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E15" s="63" t="s">
         <v>153</v>
@@ -3232,7 +3193,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
@@ -3275,7 +3236,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K16" s="68"/>
       <c r="O16" s="2" t="str">
@@ -3296,7 +3257,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E17" s="63" t="s">
         <v>153</v>
@@ -3318,7 +3279,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K17" s="66"/>
       <c r="O17" s="2" t="str">
@@ -3339,7 +3300,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E18" s="63" t="s">
         <v>153</v>
@@ -3361,7 +3322,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K18" s="66"/>
       <c r="O18" s="2" t="str">
@@ -3371,24 +3332,24 @@
     </row>
     <row r="19" spans="1:15" s="11" customFormat="1">
       <c r="A19" s="12" t="str">
-        <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>196</v>
+        <v>229</v>
       </c>
       <c r="C19" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E19" s="63" t="s">
         <v>153</v>
       </c>
       <c r="F19" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I19="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG10_small</v>
       </c>
       <c r="G19" s="13" t="str">
@@ -3396,7 +3357,7 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H19" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I19&lt;&gt;"",I19&lt;&gt;0),IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG10_zoom</v>
       </c>
       <c r="I19" s="13" t="str">
@@ -3404,7 +3365,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="67" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="K19" s="68"/>
       <c r="O19" s="2" t="str">
@@ -3414,24 +3375,24 @@
     </row>
     <row r="20" spans="1:15" s="11" customFormat="1">
       <c r="A20" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE(LEFT(A19,3),IF(MID(A19,4,2)+1&lt;10,CONCATENATE("0",MID(A19,4,2)+1),MID(A19,4,2)+1)),"")</f>
         <v>IMG11</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C20" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E20" s="63" t="s">
         <v>153</v>
       </c>
       <c r="F20" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE($C$7,"_",$A20,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I20="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG11_small</v>
       </c>
       <c r="G20" s="13" t="str">
@@ -3439,17 +3400,17 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H20" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I20&lt;&gt;"",I20&lt;&gt;0),IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE($C$7,"_",$A20,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG11_zoom</v>
       </c>
       <c r="I20" s="13" t="str">
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J20" s="64" t="s">
-        <v>215</v>
-      </c>
-      <c r="K20" s="66"/>
+      <c r="J20" s="67" t="s">
+        <v>213</v>
+      </c>
+      <c r="K20" s="68"/>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>
         <v>F10B</v>
@@ -3457,14 +3418,14 @@
     </row>
     <row r="21" spans="1:15" s="11" customFormat="1">
       <c r="A21" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE(LEFT(A20,3),IF(MID(A20,4,2)+1&lt;10,CONCATENATE("0",MID(A20,4,2)+1),MID(A20,4,2)+1)),"")</f>
         <v>IMG12</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C21" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="63" t="s">
@@ -3474,7 +3435,7 @@
         <v>153</v>
       </c>
       <c r="F21" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE($C$7,"_",$A21,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I21="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG12_small</v>
       </c>
       <c r="G21" s="13" t="str">
@@ -3482,17 +3443,19 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H21" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I21&lt;&gt;"",I21&lt;&gt;0),IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE($C$7,"_",$A21,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG12_zoom</v>
       </c>
       <c r="I21" s="13" t="str">
         <f ca="1">IF(OR($B21&lt;&gt;"",$J21&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J21" s="66" t="s">
-        <v>216</v>
-      </c>
-      <c r="K21" s="66"/>
+      <c r="J21" s="64" t="s">
+        <v>214</v>
+      </c>
+      <c r="K21" s="66" t="s">
+        <v>231</v>
+      </c>
       <c r="O21" s="2" t="str">
         <f>'Definición técnica de imagenes'!A33</f>
         <v>F11</v>
@@ -3500,14 +3463,14 @@
     </row>
     <row r="22" spans="1:15" s="11" customFormat="1">
       <c r="A22" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),CONCATENATE(LEFT(A21,3),IF(MID(A21,4,2)+1&lt;10,CONCATENATE("0",MID(A21,4,2)+1),MID(A21,4,2)+1)),"")</f>
         <v>IMG13</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C22" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="63" t="s">
@@ -3517,7 +3480,7 @@
         <v>153</v>
       </c>
       <c r="F22" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),CONCATENATE($C$7,"_",$A22,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I22="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG13_small</v>
       </c>
       <c r="G22" s="13" t="str">
@@ -3525,42 +3488,42 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H22" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I22&lt;&gt;"",I22&lt;&gt;0),IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),CONCATENATE($C$7,"_",$A22,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG13_zoom</v>
       </c>
       <c r="I22" s="13" t="str">
         <f ca="1">IF(OR($B22&lt;&gt;"",$J22&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J22" s="63" t="s">
-        <v>217</v>
-      </c>
-      <c r="K22" s="108"/>
+      <c r="J22" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="K22" s="66"/>
       <c r="O22" s="2" t="str">
         <f>'Definición técnica de imagenes'!A34</f>
         <v>F12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="23" spans="1:15" s="11" customFormat="1">
       <c r="A23" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),CONCATENATE(LEFT(A22,3),IF(MID(A22,4,2)+1&lt;10,CONCATENATE("0",MID(A22,4,2)+1),MID(A22,4,2)+1)),"")</f>
         <v>IMG14</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C23" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E23" s="63" t="s">
         <v>153</v>
       </c>
       <c r="F23" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),CONCATENATE($C$7,"_",$A23,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I23="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG14_small</v>
       </c>
       <c r="G23" s="13" t="str">
@@ -3568,17 +3531,17 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H23" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I23&lt;&gt;"",I23&lt;&gt;0),IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),CONCATENATE($C$7,"_",$A23,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG14_zoom</v>
       </c>
       <c r="I23" s="13" t="str">
         <f ca="1">IF(OR($B23&lt;&gt;"",$J23&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J23" s="64" t="s">
-        <v>218</v>
-      </c>
-      <c r="K23" s="64"/>
+      <c r="J23" s="63" t="s">
+        <v>216</v>
+      </c>
+      <c r="K23" s="77"/>
       <c r="O23" s="2" t="str">
         <f>'Definición técnica de imagenes'!A35</f>
         <v>F13</v>
@@ -3586,24 +3549,24 @@
     </row>
     <row r="24" spans="1:15" s="11" customFormat="1" ht="26">
       <c r="A24" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),CONCATENATE(LEFT(A23,3),IF(MID(A23,4,2)+1&lt;10,CONCATENATE("0",MID(A23,4,2)+1),MID(A23,4,2)+1)),"")</f>
         <v>IMG15</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C24" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D24" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E24" s="63" t="s">
         <v>153</v>
       </c>
       <c r="F24" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),CONCATENATE($C$7,"_",$A24,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I24="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG15_small</v>
       </c>
       <c r="G24" s="13" t="str">
@@ -3611,42 +3574,42 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H24" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I24&lt;&gt;"",I24&lt;&gt;0),IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),CONCATENATE($C$7,"_",$A24,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG15_zoom</v>
       </c>
       <c r="I24" s="13" t="str">
         <f ca="1">IF(OR($B24&lt;&gt;"",$J24&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J24" s="63" t="s">
-        <v>219</v>
-      </c>
-      <c r="K24" s="65"/>
+      <c r="J24" s="64" t="s">
+        <v>217</v>
+      </c>
+      <c r="K24" s="64"/>
       <c r="O24" s="2" t="str">
         <f>'Definición técnica de imagenes'!A37</f>
         <v>F13B</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" ht="52">
+    <row r="25" spans="1:15" s="11" customFormat="1" ht="26">
       <c r="A25" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),CONCATENATE(LEFT(A24,3),IF(MID(A24,4,2)+1&lt;10,CONCATENATE("0",MID(A24,4,2)+1),MID(A24,4,2)+1)),"")</f>
         <v>IMG16</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C25" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D25" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E25" s="63" t="s">
         <v>153</v>
       </c>
       <c r="F25" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),CONCATENATE($C$7,"_",$A25,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I25="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG16_small</v>
       </c>
       <c r="G25" s="13" t="str">
@@ -3654,7 +3617,7 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H25" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I25&lt;&gt;"",I25&lt;&gt;0),IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),CONCATENATE($C$7,"_",$A25,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG16_zoom</v>
       </c>
       <c r="I25" s="13" t="str">
@@ -3662,22 +3625,20 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="63" t="s">
-        <v>220</v>
-      </c>
-      <c r="K25" s="64" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="11" customFormat="1" ht="26">
+        <v>218</v>
+      </c>
+      <c r="K25" s="65"/>
+    </row>
+    <row r="26" spans="1:15" s="11" customFormat="1" ht="52">
       <c r="A26" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),CONCATENATE(LEFT(A25,3),IF(MID(A25,4,2)+1&lt;10,CONCATENATE("0",MID(A25,4,2)+1),MID(A25,4,2)+1)),"")</f>
         <v>IMG17</v>
       </c>
       <c r="B26" s="62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C26" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D26" s="63" t="s">
@@ -3687,7 +3648,7 @@
         <v>153</v>
       </c>
       <c r="F26" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),CONCATENATE($C$7,"_",$A26,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I26="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG17_small</v>
       </c>
       <c r="G26" s="13" t="str">
@@ -3695,7 +3656,7 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H26" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I26&lt;&gt;"",I26&lt;&gt;0),IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),CONCATENATE($C$7,"_",$A26,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG17_zoom</v>
       </c>
       <c r="I26" s="13" t="str">
@@ -3703,30 +3664,32 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="63" t="s">
-        <v>222</v>
-      </c>
-      <c r="K26" s="64"/>
-    </row>
-    <row r="27" spans="1:15" s="11" customFormat="1">
+        <v>219</v>
+      </c>
+      <c r="K26" s="64" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="11" customFormat="1" ht="26">
       <c r="A27" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),CONCATENATE(LEFT(A26,3),IF(MID(A26,4,2)+1&lt;10,CONCATENATE("0",MID(A26,4,2)+1),MID(A26,4,2)+1)),"")</f>
         <v>IMG18</v>
       </c>
       <c r="B27" s="62" t="s">
         <v>199</v>
       </c>
       <c r="C27" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E27" s="63" t="s">
         <v>153</v>
       </c>
       <c r="F27" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),CONCATENATE($C$7,"_",$A27,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I27="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG18_small</v>
       </c>
       <c r="G27" s="13" t="str">
@@ -3734,39 +3697,39 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H27" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I27&lt;&gt;"",I27&lt;&gt;0),IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),CONCATENATE($C$7,"_",$A27,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG18_zoom</v>
       </c>
       <c r="I27" s="13" t="str">
         <f ca="1">IF(OR($B27&lt;&gt;"",$J27&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E27,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E27,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J27" s="64" t="s">
-        <v>223</v>
+      <c r="J27" s="63" t="s">
+        <v>221</v>
       </c>
       <c r="K27" s="64"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="28" spans="1:15" s="11" customFormat="1">
       <c r="A28" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),CONCATENATE(LEFT(A27,3),IF(MID(A27,4,2)+1&lt;10,CONCATENATE("0",MID(A27,4,2)+1),MID(A27,4,2)+1)),"")</f>
         <v>IMG19</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C28" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D28" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E28" s="63" t="s">
         <v>153</v>
       </c>
       <c r="F28" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),CONCATENATE($C$7,"_",$A28,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I28="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_10_04_CO_IMG19_small</v>
       </c>
       <c r="G28" s="13" t="str">
@@ -3774,7 +3737,7 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H28" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I28&lt;&gt;"",I28&lt;&gt;0),IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),CONCATENATE($C$7,"_",$A28,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_10_04_CO_IMG19_zoom</v>
       </c>
       <c r="I28" s="13" t="str">
@@ -3782,24 +3745,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J28" s="64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" ht="65">
+    <row r="29" spans="1:15" s="11" customFormat="1" ht="26">
       <c r="A29" s="12" t="str">
         <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),CONCATENATE(LEFT(A28,3),IF(MID(A28,4,2)+1&lt;10,CONCATENATE("0",MID(A28,4,2)+1),MID(A28,4,2)+1)),"")</f>
         <v>IMG20</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C29" s="20" t="str">
         <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D29" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E29" s="63" t="s">
         <v>153</v>
@@ -3821,26 +3784,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J29" s="64" t="s">
-        <v>225</v>
-      </c>
-      <c r="K29" s="64" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" ht="26">
+        <v>223</v>
+      </c>
+      <c r="K29" s="64"/>
+    </row>
+    <row r="30" spans="1:15" s="11" customFormat="1" ht="65">
       <c r="A30" s="12" t="str">
         <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),CONCATENATE(LEFT(A29,3),IF(MID(A29,4,2)+1&lt;10,CONCATENATE("0",MID(A29,4,2)+1),MID(A29,4,2)+1)),"")</f>
         <v>IMG21</v>
       </c>
       <c r="B30" s="62" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C30" s="20" t="str">
         <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D30" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E30" s="63" t="s">
         <v>153</v>
@@ -3862,19 +3823,19 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J30" s="64" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K30" s="64" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="11" customFormat="1" ht="26">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="11" customFormat="1">
       <c r="A31" s="12" t="str">
         <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),CONCATENATE(LEFT(A30,3),IF(MID(A30,4,2)+1&lt;10,CONCATENATE("0",MID(A30,4,2)+1),MID(A30,4,2)+1)),"")</f>
         <v>IMG22</v>
       </c>
       <c r="B31" s="62" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C31" s="20" t="str">
         <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -3903,7 +3864,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J31" s="64" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="K31" s="64"/>
     </row>
@@ -3913,14 +3874,14 @@
         <v>IMG23</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="C32" s="20" t="str">
         <f>IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D32" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E32" s="63" t="s">
         <v>153</v>
@@ -3942,546 +3903,432 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J32" s="64" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="K32" s="64" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="11" customFormat="1" ht="26">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="11" customFormat="1">
       <c r="A33" s="12" t="str">
         <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),CONCATENATE(LEFT(A32,3),IF(MID(A32,4,2)+1&lt;10,CONCATENATE("0",MID(A32,4,2)+1),MID(A32,4,2)+1)),"")</f>
-        <v>IMG24</v>
-      </c>
-      <c r="B33" s="62" t="s">
-        <v>227</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B33" s="62"/>
       <c r="C33" s="20" t="str">
         <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D33" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E33" s="63" t="s">
-        <v>153</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
       <c r="F33" s="13" t="str">
         <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),CONCATENATE($C$7,"_",$A33,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I33="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_10_04_CO_IMG24_small</v>
+        <v/>
       </c>
       <c r="G33" s="13" t="str">
         <f ca="1">IF($F33&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E33,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H33" s="13" t="str">
         <f ca="1">IF(AND(I33&lt;&gt;"",I33&lt;&gt;0),IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),CONCATENATE($C$7,"_",$A33,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_10_04_CO_IMG24_zoom</v>
+        <v/>
       </c>
       <c r="I33" s="13" t="str">
         <f ca="1">IF(OR($B33&lt;&gt;"",$J33&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E33,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E33,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J33" s="64" t="s">
-        <v>238</v>
-      </c>
-      <c r="K33" s="64" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="11" customFormat="1" ht="117">
+        <v/>
+      </c>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
+    </row>
+    <row r="34" spans="1:15" s="11" customFormat="1">
       <c r="A34" s="12" t="str">
         <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE(LEFT(A33,3),IF(MID(A33,4,2)+1&lt;10,CONCATENATE("0",MID(A33,4,2)+1),MID(A33,4,2)+1)),"")</f>
-        <v>IMG25</v>
-      </c>
-      <c r="B34" s="62" t="s">
-        <v>228</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B34" s="62"/>
       <c r="C34" s="20" t="str">
         <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D34" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E34" s="63" t="s">
-        <v>153</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
       <c r="F34" s="13" t="str">
         <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE($C$7,"_",$A34,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I34="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_10_04_CO_IMG25_small</v>
+        <v/>
       </c>
       <c r="G34" s="13" t="str">
         <f ca="1">IF($F34&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E34,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H34" s="13" t="str">
         <f ca="1">IF(AND(I34&lt;&gt;"",I34&lt;&gt;0),IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE($C$7,"_",$A34,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_10_04_CO_IMG25_zoom</v>
+        <v/>
       </c>
       <c r="I34" s="13" t="str">
         <f ca="1">IF(OR($B34&lt;&gt;"",$J34&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E34,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E34,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J34" s="64" t="s">
-        <v>230</v>
-      </c>
-      <c r="K34" s="64" t="s">
-        <v>240</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="35" spans="1:15" s="11" customFormat="1">
       <c r="A35" s="12" t="str">
         <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),CONCATENATE(LEFT(A34,3),IF(MID(A34,4,2)+1&lt;10,CONCATENATE("0",MID(A34,4,2)+1),MID(A34,4,2)+1)),"")</f>
-        <v>IMG26</v>
-      </c>
-      <c r="B35" s="62" t="s">
-        <v>228</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B35" s="62"/>
       <c r="C35" s="20" t="str">
         <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D35" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E35" s="63" t="s">
-        <v>153</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
       <c r="F35" s="13" t="str">
         <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),CONCATENATE($C$7,"_",$A35,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I35="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_10_04_CO_IMG26_small</v>
+        <v/>
       </c>
       <c r="G35" s="13" t="str">
         <f ca="1">IF($F35&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E35,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H35" s="13" t="str">
         <f ca="1">IF(AND(I35&lt;&gt;"",I35&lt;&gt;0),IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),CONCATENATE($C$7,"_",$A35,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_10_04_CO_IMG26_zoom</v>
+        <v/>
       </c>
       <c r="I35" s="13" t="str">
         <f ca="1">IF(OR($B35&lt;&gt;"",$J35&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E35,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E35,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J35" s="64" t="s">
-        <v>231</v>
-      </c>
-      <c r="K35" s="64" t="s">
-        <v>239</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="36" spans="1:15" s="11" customFormat="1">
       <c r="A36" s="12" t="str">
         <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),CONCATENATE(LEFT(A35,3),IF(MID(A35,4,2)+1&lt;10,CONCATENATE("0",MID(A35,4,2)+1),MID(A35,4,2)+1)),"")</f>
-        <v>IMG27</v>
-      </c>
-      <c r="B36" s="62" t="s">
-        <v>242</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B36" s="62"/>
       <c r="C36" s="20" t="str">
         <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D36" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E36" s="63" t="s">
-        <v>153</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
       <c r="F36" s="13" t="str">
         <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),CONCATENATE($C$7,"_",$A36,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I36="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_10_04_CO_IMG27_small</v>
+        <v/>
       </c>
       <c r="G36" s="13" t="str">
         <f ca="1">IF($F36&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E36,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H36" s="13" t="str">
         <f ca="1">IF(AND(I36&lt;&gt;"",I36&lt;&gt;0),IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),CONCATENATE($C$7,"_",$A36,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_10_04_CO_IMG27_zoom</v>
+        <v/>
       </c>
       <c r="I36" s="13" t="str">
         <f ca="1">IF(OR($B36&lt;&gt;"",$J36&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E36,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E36,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J36" s="63" t="s">
-        <v>241</v>
-      </c>
-      <c r="K36" s="65"/>
+        <v/>
+      </c>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="37" spans="1:15" s="11" customFormat="1">
       <c r="A37" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG28</v>
-      </c>
-      <c r="B37" s="62" t="s">
-        <v>242</v>
-      </c>
+        <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),CONCATENATE(LEFT(A36,3),IF(MID(A36,4,2)+1&lt;10,CONCATENATE("0",MID(A36,4,2)+1),MID(A36,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B37" s="62"/>
       <c r="C37" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D37" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E37" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
       <c r="F37" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG28_small</v>
+        <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),CONCATENATE($C$7,"_",$A37,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I37="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G37" s="13" t="str">
         <f ca="1">IF($F37&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E37,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H37" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG28_zoom</v>
+        <f ca="1">IF(AND(I37&lt;&gt;"",I37&lt;&gt;0),IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),CONCATENATE($C$7,"_",$A37,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I37" s="13" t="str">
         <f ca="1">IF(OR($B37&lt;&gt;"",$J37&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E37,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E37,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J37" s="69" t="s">
-        <v>243</v>
-      </c>
-      <c r="K37" s="65"/>
+        <v/>
+      </c>
+      <c r="J37" s="64"/>
+      <c r="K37" s="64"/>
     </row>
     <row r="38" spans="1:15" s="11" customFormat="1">
       <c r="A38" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG29</v>
-      </c>
-      <c r="B38" s="62" t="s">
-        <v>245</v>
-      </c>
+        <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),CONCATENATE(LEFT(A37,3),IF(MID(A37,4,2)+1&lt;10,CONCATENATE("0",MID(A37,4,2)+1),MID(A37,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B38" s="62"/>
       <c r="C38" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D38" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E38" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
       <c r="F38" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG29_small</v>
+        <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),CONCATENATE($C$7,"_",$A38,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I38="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G38" s="13" t="str">
         <f ca="1">IF($F38&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E38,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H38" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG29_zoom</v>
+        <f ca="1">IF(AND(I38&lt;&gt;"",I38&lt;&gt;0),IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),CONCATENATE($C$7,"_",$A38,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I38" s="13" t="str">
         <f ca="1">IF(OR($B38&lt;&gt;"",$J38&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E38,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E38,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J38" s="70" t="s">
-        <v>244</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J38" s="63"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:15" s="11" customFormat="1" ht="65">
+    <row r="39" spans="1:15" s="11" customFormat="1">
       <c r="A39" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG30</v>
-      </c>
-      <c r="B39" s="62" t="s">
-        <v>246</v>
-      </c>
+        <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),CONCATENATE(LEFT(A38,3),IF(MID(A38,4,2)+1&lt;10,CONCATENATE("0",MID(A38,4,2)+1),MID(A38,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B39" s="62"/>
       <c r="C39" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D39" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E39" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
       <c r="F39" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG30_small</v>
+        <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),CONCATENATE($C$7,"_",$A39,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I39="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G39" s="13" t="str">
         <f ca="1">IF($F39&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E39,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H39" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG30_zoom</v>
+        <f ca="1">IF(AND(I39&lt;&gt;"",I39&lt;&gt;0),IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),CONCATENATE($C$7,"_",$A39,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I39" s="13" t="str">
         <f ca="1">IF(OR($B39&lt;&gt;"",$J39&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E39,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E39,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J39" s="63" t="s">
-        <v>247</v>
-      </c>
-      <c r="K39" s="65" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" s="11" customFormat="1" ht="39">
+        <v/>
+      </c>
+      <c r="J39" s="69"/>
+      <c r="K39" s="65"/>
+    </row>
+    <row r="40" spans="1:15" s="11" customFormat="1">
       <c r="A40" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG31</v>
-      </c>
-      <c r="B40" s="62" t="s">
-        <v>250</v>
-      </c>
+        <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),CONCATENATE(LEFT(A39,3),IF(MID(A39,4,2)+1&lt;10,CONCATENATE("0",MID(A39,4,2)+1),MID(A39,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B40" s="62"/>
       <c r="C40" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D40" s="63" t="s">
-        <v>187</v>
-      </c>
-      <c r="E40" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
       <c r="F40" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG31_small</v>
+        <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),CONCATENATE($C$7,"_",$A40,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I40="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G40" s="13" t="str">
         <f ca="1">IF($F40&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E40,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H40" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG31_zoom</v>
+        <f ca="1">IF(AND(I40&lt;&gt;"",I40&lt;&gt;0),IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),CONCATENATE($C$7,"_",$A40,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I40" s="13" t="str">
         <f ca="1">IF(OR($B40&lt;&gt;"",$J40&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E40,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E40,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J40" s="63" t="s">
-        <v>249</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J40" s="70"/>
       <c r="K40" s="65"/>
     </row>
     <row r="41" spans="1:15" s="11" customFormat="1">
       <c r="A41" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG32</v>
-      </c>
-      <c r="B41" s="62" t="s">
-        <v>252</v>
-      </c>
+        <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE(LEFT(A40,3),IF(MID(A40,4,2)+1&lt;10,CONCATENATE("0",MID(A40,4,2)+1),MID(A40,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B41" s="62"/>
       <c r="C41" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D41" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E41" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
       <c r="F41" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG32_small</v>
+        <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE($C$7,"_",$A41,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I41="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G41" s="13" t="str">
         <f ca="1">IF($F41&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E41,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H41" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG32_zoom</v>
+        <f ca="1">IF(AND(I41&lt;&gt;"",I41&lt;&gt;0),IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE($C$7,"_",$A41,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I41" s="13" t="str">
         <f ca="1">IF(OR($B41&lt;&gt;"",$J41&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E41,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E41,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J41" s="63" t="s">
-        <v>251</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J41" s="63"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="42" spans="1:15" s="11" customFormat="1">
       <c r="A42" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG33</v>
-      </c>
-      <c r="B42" s="62" t="s">
-        <v>254</v>
-      </c>
+        <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),CONCATENATE(LEFT(A41,3),IF(MID(A41,4,2)+1&lt;10,CONCATENATE("0",MID(A41,4,2)+1),MID(A41,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B42" s="62"/>
       <c r="C42" s="20" t="str">
-        <f t="shared" ref="C42:C73" si="7">IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D42" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E42" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
       <c r="F42" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG33_small</v>
+        <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),CONCATENATE($C$7,"_",$A42,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I42="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G42" s="13" t="str">
         <f ca="1">IF($F42&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E42,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H42" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG33_zoom</v>
+        <f ca="1">IF(AND(I42&lt;&gt;"",I42&lt;&gt;0),IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),CONCATENATE($C$7,"_",$A42,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I42" s="13" t="str">
         <f ca="1">IF(OR($B42&lt;&gt;"",$J42&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E42,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E42,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J42" s="63" t="s">
-        <v>253</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="43" spans="1:15" s="11" customFormat="1">
       <c r="A43" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG34</v>
-      </c>
-      <c r="B43" s="62" t="s">
-        <v>256</v>
-      </c>
+        <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),CONCATENATE(LEFT(A42,3),IF(MID(A42,4,2)+1&lt;10,CONCATENATE("0",MID(A42,4,2)+1),MID(A42,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B43" s="62"/>
       <c r="C43" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D43" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E43" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
       <c r="F43" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG34_small</v>
+        <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),CONCATENATE($C$7,"_",$A43,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I43="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G43" s="13" t="str">
         <f ca="1">IF($F43&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E43,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H43" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG34_zoom</v>
+        <f ca="1">IF(AND(I43&lt;&gt;"",I43&lt;&gt;0),IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),CONCATENATE($C$7,"_",$A43,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I43" s="13" t="str">
         <f ca="1">IF(OR($B43&lt;&gt;"",$J43&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E43,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E43,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J43" s="63" t="s">
-        <v>255</v>
-      </c>
-      <c r="K43" s="65" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" s="11" customFormat="1" ht="26">
+        <v/>
+      </c>
+      <c r="J43" s="63"/>
+      <c r="K43" s="65"/>
+    </row>
+    <row r="44" spans="1:15" s="11" customFormat="1">
       <c r="A44" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG35</v>
-      </c>
-      <c r="B44" s="62" t="s">
-        <v>259</v>
-      </c>
+        <f>IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),CONCATENATE(LEFT(A43,3),IF(MID(A43,4,2)+1&lt;10,CONCATENATE("0",MID(A43,4,2)+1),MID(A43,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B44" s="62"/>
       <c r="C44" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D44" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E44" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
       <c r="F44" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG35_small</v>
+        <f>IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),CONCATENATE($C$7,"_",$A44,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I44="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G44" s="13" t="str">
         <f ca="1">IF($F44&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E44,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H44" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG35_zoom</v>
+        <f ca="1">IF(AND(I44&lt;&gt;"",I44&lt;&gt;0),IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),CONCATENATE($C$7,"_",$A44,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I44" s="13" t="str">
         <f ca="1">IF(OR($B44&lt;&gt;"",$J44&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E44,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E44,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J44" s="63" t="s">
-        <v>258</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J44" s="63"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:15" s="11" customFormat="1" ht="26">
+    <row r="45" spans="1:15" s="11" customFormat="1">
       <c r="A45" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v>IMG36</v>
-      </c>
-      <c r="B45" s="62" t="s">
-        <v>259</v>
-      </c>
+        <f>IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),CONCATENATE(LEFT(A44,3),IF(MID(A44,4,2)+1&lt;10,CONCATENATE("0",MID(A44,4,2)+1),MID(A44,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B45" s="62"/>
       <c r="C45" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D45" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" s="63" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
       <c r="F45" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>CN_10_04_CO_IMG36_small</v>
+        <f>IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),CONCATENATE($C$7,"_",$A45,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I45="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G45" s="13" t="str">
         <f ca="1">IF($F45&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E45,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H45" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>CN_10_04_CO_IMG36_zoom</v>
+        <f ca="1">IF(AND(I45&lt;&gt;"",I45&lt;&gt;0),IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),CONCATENATE($C$7,"_",$A45,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v/>
       </c>
       <c r="I45" s="13" t="str">
         <f ca="1">IF(OR($B45&lt;&gt;"",$J45&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E45,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E45,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J45" s="63" t="s">
-        <v>260</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J45" s="63"/>
       <c r="K45" s="65"/>
     </row>
     <row r="46" spans="1:15" s="11" customFormat="1">
       <c r="A46" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),CONCATENATE(LEFT(A45,3),IF(MID(A45,4,2)+1&lt;10,CONCATENATE("0",MID(A45,4,2)+1),MID(A45,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B46" s="62"/>
       <c r="C46" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D46" s="63"/>
       <c r="E46" s="63"/>
       <c r="F46" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),CONCATENATE($C$7,"_",$A46,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I46="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G46" s="13" t="str">
@@ -4489,7 +4336,7 @@
         <v/>
       </c>
       <c r="H46" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">IF(AND(I46&lt;&gt;"",I46&lt;&gt;0),IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),CONCATENATE($C$7,"_",$A46,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I46" s="13" t="str">
@@ -4501,12 +4348,12 @@
     </row>
     <row r="47" spans="1:15" s="11" customFormat="1">
       <c r="A47" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A47:A50" si="6">IF(OR(B47&lt;&gt;"",J47&lt;&gt;""),CONCATENATE(LEFT(A46,3),IF(MID(A46,4,2)+1&lt;10,CONCATENATE("0",MID(A46,4,2)+1),MID(A46,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B47" s="62"/>
       <c r="C47" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="C47:C73" si="7">IF(OR(B47&lt;&gt;"",J47&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D47" s="63"/>
@@ -6492,25 +6339,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" thickBot="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="95"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="98"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -6518,11 +6365,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="104"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6573,11 +6420,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="104" t="str">
+      <c r="D5" s="105" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="105"/>
+      <c r="E5" s="106"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6622,12 +6469,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="90" t="str">
+      <c r="D7" s="91" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6721,14 +6568,14 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="95"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6761,12 +6608,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6806,12 +6653,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="98" t="str">
+      <c r="D17" s="99" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="101"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6827,12 +6674,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="90" t="str">
+      <c r="D18" s="91" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="90"/>
-      <c r="F18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="92"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -7236,40 +7083,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="108" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="107" t="s">
+      <c r="E1" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="G1" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="106"/>
+      <c r="I1" s="107"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>

</xml_diff>